<commit_message>
MAJ Documentation codes FIP 25.00.00
</commit_message>
<xml_diff>
--- a/Noyau RH FPE/6. NOMENCLATURES ET AUTRES REFERENTIELS/Nomenclatures SIRH/Informations complémentaires/FIP_CONGE_ABSENCE_25.00.00.xlsx
+++ b/Noyau RH FPE/6. NOMENCLATURES ET AUTRES REFERENTIELS/Nomenclatures SIRH/Informations complémentaires/FIP_CONGE_ABSENCE_25.00.00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\BALIDFS1\onp\ONP\CISIRH\03-BARRI\REFERENTIELS\NOYAU\1-20250704_25.00.00\8-Informations complémentaires\Correspondance codes FIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\03-BARRI\VERSIONS NOYAU DIFFUSEES\20250704_25.00.00\8-Informations complémentaires\Correspondance codes FIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D371224-E2DE-4D01-8BE6-E5193B55542D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07977DC-38F8-4805-9AC7-F244F5A57A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="170" windowWidth="14280" windowHeight="10080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONGE_ABSENCE" sheetId="1" r:id="rId1"/>
@@ -2349,8 +2349,8 @@
   <dimension ref="A1:J171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3323,8 +3323,8 @@
       <c r="H38" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="40" t="s">
-        <v>116</v>
+      <c r="I38" s="31" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>